<commit_message>
Updated AVGO and MRVL data to the latest quarter
</commit_message>
<xml_diff>
--- a/data/AVGO.xlsx
+++ b/data/AVGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B59CD-31BD-4AAC-8051-85A9D52F7E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A35363-5815-469E-A9AB-6B9423D7406B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="4210" windowWidth="28800" windowHeight="15370" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
+    <workbookView xWindow="5500" yWindow="5180" windowWidth="38380" windowHeight="9890" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Infrastructure Software</t>
   </si>
@@ -50,28 +50,37 @@
     <t>Reporting Quarter</t>
   </si>
   <si>
-    <t>Q1 '23</t>
-  </si>
-  <si>
-    <t>Q2 '23</t>
-  </si>
-  <si>
-    <t>Q3 '23</t>
-  </si>
-  <si>
-    <t>Q4 '23</t>
-  </si>
-  <si>
-    <t>Q1 '24</t>
-  </si>
-  <si>
-    <t>Q2 '24</t>
-  </si>
-  <si>
-    <t>Q3 '24</t>
-  </si>
-  <si>
-    <t>Q4 '24</t>
+    <t>Q1 FY23</t>
+  </si>
+  <si>
+    <t>Q2 FY23</t>
+  </si>
+  <si>
+    <t>Q3 FY23</t>
+  </si>
+  <si>
+    <t>Q4 FY23</t>
+  </si>
+  <si>
+    <t>Q1 FY24</t>
+  </si>
+  <si>
+    <t>Q2 FY24</t>
+  </si>
+  <si>
+    <t>Q3 FY24</t>
+  </si>
+  <si>
+    <t>Q4 FY24</t>
+  </si>
+  <si>
+    <t>Q1 FY25</t>
+  </si>
+  <si>
+    <t>Q2 FY25</t>
+  </si>
+  <si>
+    <t>Q3 FY25</t>
   </si>
 </sst>
 </file>
@@ -445,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7699876-666C-41D6-B24A-347A2FC5C849}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,7 +469,7 @@
     <col min="9" max="9" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -488,8 +497,17 @@
       <c r="I1" t="s">
         <v>11</v>
       </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -517,8 +535,17 @@
       <c r="I2" s="1">
         <v>45599</v>
       </c>
+      <c r="J2" s="1">
+        <v>45690</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45781</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45872</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -546,8 +573,17 @@
       <c r="I3" s="2">
         <v>8230</v>
       </c>
+      <c r="J3" s="2">
+        <v>8212</v>
+      </c>
+      <c r="K3" s="2">
+        <v>8408</v>
+      </c>
+      <c r="L3" s="2">
+        <v>9166</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -574,6 +610,15 @@
       </c>
       <c r="I4" s="2">
         <v>5824</v>
+      </c>
+      <c r="J4" s="2">
+        <v>6704</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6596</v>
+      </c>
+      <c r="L4" s="2">
+        <v>6786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>